<commit_message>
Add in decision handling for day
</commit_message>
<xml_diff>
--- a/tests/usdm4/test_files/expander/example_study.xlsx
+++ b/tests/usdm4/test_files/expander/example_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/github/usdm4/tests/usdm4/test_files/expander/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111B6BFD-28C6-1D4D-BDF7-70613ABE9DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC83318-37F9-BF4F-A5BC-AD264ABFCA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" firstSheet="6" activeTab="7" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" firstSheet="17" activeTab="18" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -30,23 +30,24 @@
     <sheet name="earlyTerminationTimeline" sheetId="23" r:id="rId15"/>
     <sheet name="vsBloodPressure" sheetId="24" r:id="rId16"/>
     <sheet name="extra" sheetId="35" r:id="rId17"/>
-    <sheet name="studyDesignTiming" sheetId="18" r:id="rId18"/>
-    <sheet name="studyDesignConditions" sheetId="27" r:id="rId19"/>
-    <sheet name="studyDesignActivities" sheetId="21" r:id="rId20"/>
-    <sheet name="studyDesignInterventions" sheetId="25" r:id="rId21"/>
-    <sheet name="studyDesignIndications" sheetId="6" r:id="rId22"/>
-    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId23"/>
-    <sheet name="studyDesignOE" sheetId="8" r:id="rId24"/>
-    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId25"/>
-    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId26"/>
-    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId27"/>
-    <sheet name="studyDesignElements" sheetId="13" r:id="rId28"/>
-    <sheet name="dictionaries" sheetId="20" r:id="rId29"/>
-    <sheet name="roles" sheetId="31" r:id="rId30"/>
-    <sheet name="lillyFormat" sheetId="16" r:id="rId31"/>
-    <sheet name="m11Format" sheetId="28" r:id="rId32"/>
-    <sheet name="documentContent" sheetId="29" r:id="rId33"/>
-    <sheet name="configuration" sheetId="10" r:id="rId34"/>
+    <sheet name="dayCycle" sheetId="36" r:id="rId18"/>
+    <sheet name="studyDesignTiming" sheetId="18" r:id="rId19"/>
+    <sheet name="studyDesignConditions" sheetId="27" r:id="rId20"/>
+    <sheet name="studyDesignActivities" sheetId="21" r:id="rId21"/>
+    <sheet name="studyDesignInterventions" sheetId="25" r:id="rId22"/>
+    <sheet name="studyDesignIndications" sheetId="6" r:id="rId23"/>
+    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId24"/>
+    <sheet name="studyDesignOE" sheetId="8" r:id="rId25"/>
+    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId26"/>
+    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId27"/>
+    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId28"/>
+    <sheet name="studyDesignElements" sheetId="13" r:id="rId29"/>
+    <sheet name="dictionaries" sheetId="20" r:id="rId30"/>
+    <sheet name="roles" sheetId="31" r:id="rId31"/>
+    <sheet name="lillyFormat" sheetId="16" r:id="rId32"/>
+    <sheet name="m11Format" sheetId="28" r:id="rId33"/>
+    <sheet name="documentContent" sheetId="29" r:id="rId34"/>
+    <sheet name="configuration" sheetId="10" r:id="rId35"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3356" uniqueCount="1581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3441" uniqueCount="1606">
   <si>
     <t>Screening</t>
   </si>
@@ -6872,9 +6873,6 @@
     <t>timeline</t>
   </si>
   <si>
-    <t>adverseEventTimeline, earlyTerminationTimeline, vsBloodPressure, extra</t>
-  </si>
-  <si>
     <t>EXTRA_1</t>
   </si>
   <si>
@@ -6936,6 +6934,84 @@
   </si>
   <si>
     <t>extra</t>
+  </si>
+  <si>
+    <t>Diary</t>
+  </si>
+  <si>
+    <t>DIARY_1</t>
+  </si>
+  <si>
+    <t>DIARY_2</t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>DIARY_3</t>
+  </si>
+  <si>
+    <t>DIARY_4</t>
+  </si>
+  <si>
+    <t>DIARY_5</t>
+  </si>
+  <si>
+    <t>TIM28</t>
+  </si>
+  <si>
+    <t>TIM29</t>
+  </si>
+  <si>
+    <t>TIM30</t>
+  </si>
+  <si>
+    <t>TIM31</t>
+  </si>
+  <si>
+    <t>TIM32</t>
+  </si>
+  <si>
+    <t>Diary 1</t>
+  </si>
+  <si>
+    <t>Diary 2</t>
+  </si>
+  <si>
+    <t>Diary 3</t>
+  </si>
+  <si>
+    <t>Diary 4</t>
+  </si>
+  <si>
+    <t>Diary 5</t>
+  </si>
+  <si>
+    <t>0 Days</t>
+  </si>
+  <si>
+    <t>adverseEventTimeline, earlyTerminationTimeline, vsBloodPressure, extra, dayCycle</t>
+  </si>
+  <si>
+    <t>dayCycle</t>
+  </si>
+  <si>
+    <t>DIARY_2: day &lt; 30</t>
+  </si>
+  <si>
+    <t>SOG Diary</t>
+  </si>
+  <si>
+    <t>PR: SOG Diary</t>
+  </si>
+  <si>
+    <t>Diary Timeline</t>
+  </si>
+  <si>
+    <t>Wait a day</t>
+  </si>
+  <si>
+    <t>Exit</t>
   </si>
 </sst>
 </file>
@@ -7099,7 +7175,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -7307,6 +7383,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -8701,8 +8780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:V74"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9139,8 +9218,11 @@
       <c r="C9" s="14" t="s">
         <v>1558</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>1599</v>
+      </c>
       <c r="H9" s="1" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="K9" s="54"/>
       <c r="M9" s="54"/>
@@ -10247,7 +10329,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="C32" s="4"/>
       <c r="F32" s="2"/>
@@ -10546,7 +10628,7 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="26"/>
@@ -10615,7 +10697,7 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="4"/>
@@ -12886,19 +12968,19 @@
         <v>73</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>215</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1559</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1560</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1561</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1562</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12906,7 +12988,7 @@
         <v>75</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>31</v>
@@ -12924,13 +13006,13 @@
         <v>232</v>
       </c>
       <c r="D3" s="40" t="s">
+        <v>1562</v>
+      </c>
+      <c r="E3" s="41" t="s">
         <v>1563</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="F3" s="41" t="s">
         <v>1564</v>
-      </c>
-      <c r="F3" s="41" t="s">
-        <v>1565</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -12956,10 +13038,10 @@
         <v>284</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>1560</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>1561</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>1562</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>300</v>
@@ -13133,11 +13215,314 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86FF706F-AE10-6E4B-8EAD-DB97659AF4F7}">
+  <dimension ref="A1:H30"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="53.6640625" style="1" customWidth="1"/>
+    <col min="4" max="7" width="16" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1603</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1581</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1582</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1584</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1585</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>1575</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>1562</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>1604</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>1583</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>1583</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1582</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1584</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>1585</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>1586</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="14" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="14" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="3" t="s">
+        <v>1601</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>1602</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B8B105-0AE3-CA42-845E-0FC79C427790}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13837,49 +14222,49 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>277</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>280</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>268</v>
@@ -13887,283 +14272,160 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>280</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>268</v>
       </c>
     </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>1587</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>1592</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>1592</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>1581</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>1597</v>
+      </c>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>1593</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>1593</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>1582</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>1589</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>1594</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>1594</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>1584</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>1582</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>1595</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>1595</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>1585</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>1584</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>1596</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>1596</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>1586</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>1585</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8C14B1-8C62-2C45-8CB1-1E9EDDA367B1}">
-  <dimension ref="A1:F24"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="45.83203125" customWidth="1"/>
-    <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="51" style="25" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>217</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>514</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>516</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>831</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>832</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>830</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
-        <v>833</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>835</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>834</v>
-      </c>
-      <c r="D3" s="49" t="s">
-        <v>836</v>
-      </c>
-      <c r="E3" s="48" t="s">
-        <v>288</v>
-      </c>
-      <c r="F3" s="48" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14264,6 +14526,257 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8C14B1-8C62-2C45-8CB1-1E9EDDA367B1}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="51" style="25" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>514</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>831</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="48" t="s">
+        <v>833</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>835</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>834</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>836</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>288</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4305555-B5C2-8349-A6D3-AA57DAC0BCD5}">
   <dimension ref="A1:C37"/>
   <sheetViews>
@@ -14582,7 +15095,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807AE9D8-8C9D-644F-8552-6E66F0115CF1}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -14768,7 +15281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46FA45D-9570-C643-AC7B-6310BD62121C}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -14831,7 +15344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8C2F56-38DA-1440-8447-6C36029D01F5}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -14912,7 +15425,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9162AE3F-0A5D-824F-8BC1-E6A493EFAA49}">
   <dimension ref="A1:O22"/>
   <sheetViews>
@@ -15369,7 +15882,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D036654E-7FF8-D440-BC0A-D74BC57BB3C9}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -15460,12 +15973,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29E6393-3A18-464C-A40D-B41879707264}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15631,13 +16144,27 @@
         <v>486</v>
       </c>
     </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1601</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1601</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1601</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>486</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB4E9D5-B601-284A-9651-0AA604C2B9D1}">
   <dimension ref="A1:I13"/>
   <sheetViews>
@@ -15981,7 +16508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FA5DC6-70BE-E845-A085-20526138A835}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -16122,143 +16649,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989384DC-1C54-514A-8A1E-ADD84D891BA4}">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" customWidth="1"/>
-    <col min="7" max="7" width="64.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>319</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>320</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>318</v>
-      </c>
-      <c r="B2" t="s">
-        <v>322</v>
-      </c>
-      <c r="C2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E2" t="s">
-        <v>325</v>
-      </c>
-      <c r="F2" t="s">
-        <v>326</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>1540</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
-        <v>327</v>
-      </c>
-      <c r="E3" t="s">
-        <v>325</v>
-      </c>
-      <c r="F3" t="s">
-        <v>326</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>1541</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
-        <v>417</v>
-      </c>
-      <c r="E4" t="s">
-        <v>325</v>
-      </c>
-      <c r="F4" t="s">
-        <v>326</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>418</v>
-      </c>
-      <c r="B5" t="s">
-        <v>419</v>
-      </c>
-      <c r="C5" t="s">
-        <v>420</v>
-      </c>
-      <c r="D5" t="s">
-        <v>421</v>
-      </c>
-      <c r="E5" t="s">
-        <v>299</v>
-      </c>
-      <c r="F5" t="s">
-        <v>422</v>
-      </c>
-      <c r="G5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="51"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51" t="s">
-        <v>841</v>
-      </c>
-      <c r="E6" s="51" t="s">
-        <v>299</v>
-      </c>
-      <c r="F6" s="51" t="s">
-        <v>423</v>
-      </c>
-      <c r="G6" s="51" t="s">
-        <v>232</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -16312,6 +16702,143 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989384DC-1C54-514A-8A1E-ADD84D891BA4}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="64.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E2" t="s">
+        <v>325</v>
+      </c>
+      <c r="F2" t="s">
+        <v>326</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E3" t="s">
+        <v>325</v>
+      </c>
+      <c r="F3" t="s">
+        <v>326</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>417</v>
+      </c>
+      <c r="E4" t="s">
+        <v>325</v>
+      </c>
+      <c r="F4" t="s">
+        <v>326</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>418</v>
+      </c>
+      <c r="B5" t="s">
+        <v>419</v>
+      </c>
+      <c r="C5" t="s">
+        <v>420</v>
+      </c>
+      <c r="D5" t="s">
+        <v>421</v>
+      </c>
+      <c r="E5" t="s">
+        <v>299</v>
+      </c>
+      <c r="F5" t="s">
+        <v>422</v>
+      </c>
+      <c r="G5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="51"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51" t="s">
+        <v>841</v>
+      </c>
+      <c r="E6" s="51" t="s">
+        <v>299</v>
+      </c>
+      <c r="F6" s="51" t="s">
+        <v>423</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666D5CD6-DF98-6447-9150-7AA4E8F8C9F3}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -16376,7 +16903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:F77"/>
   <sheetViews>
@@ -17939,7 +18466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E75AA97-4922-F248-8DDB-BFD2366D5770}">
   <dimension ref="A1:F156"/>
   <sheetViews>
@@ -20789,7 +21316,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3AB5D9-1FE9-BF4A-BE82-FD043736B8E5}">
   <dimension ref="A1:B86"/>
   <sheetViews>
@@ -21485,7 +22012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED6534B-B4C9-924A-BB14-180C2C37C6F1}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -21831,8 +22358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AA03AF-8646-874D-935F-A73550A0FA0C}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:F12"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21980,7 +22507,7 @@
         <v>72</v>
       </c>
       <c r="B12" s="71" t="s">
-        <v>1559</v>
+        <v>1598</v>
       </c>
       <c r="C12" s="71"/>
       <c r="D12" s="71"/>

</xml_diff>